<commit_message>
EDA and preprocessing code update
</commit_message>
<xml_diff>
--- a/Jerry/statistic.xlsx
+++ b/Jerry/statistic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiarui\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\repo\MAST30034FinalProject\Jerry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D58E5D-448A-48C0-8304-0901D9E01610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1611AF-E2FC-44A8-9B53-BFCA5F44EE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6610" yWindow="150" windowWidth="19200" windowHeight="10790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2770" yWindow="3310" windowWidth="19200" windowHeight="10790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,10 +133,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -434,24 +434,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -490,25 +490,25 @@
         <v>4</v>
       </c>
       <c r="C3">
+        <v>0.61</v>
+      </c>
+      <c r="D3">
+        <v>0.62</v>
+      </c>
+      <c r="E3">
+        <v>0.63</v>
+      </c>
+      <c r="F3">
         <v>0.6</v>
       </c>
-      <c r="D3">
-        <v>0.6</v>
-      </c>
-      <c r="E3">
-        <v>0.6</v>
-      </c>
-      <c r="F3">
-        <v>0.59</v>
-      </c>
       <c r="G3">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="H3">
-        <v>0.59</v>
+        <v>0.61</v>
       </c>
       <c r="I3">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update statistic table, with 6 significant figures
Final BERT model's result is still required
</commit_message>
<xml_diff>
--- a/Jerry/statistic.xlsx
+++ b/Jerry/statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\repo\MAST30034FinalProject\Jerry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1611AF-E2FC-44A8-9B53-BFCA5F44EE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E9BCD6-AFD0-4A5A-9108-3C5119A93C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2770" yWindow="3310" windowWidth="19200" windowHeight="10790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t xml:space="preserve"> precision</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,14 +59,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sarcasm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>not sarcasm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>recall</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -75,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BERT encoder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>feature extraction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,6 +76,22 @@
   </si>
   <si>
     <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BERT embedding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sarcastic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not sarcastic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -119,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -127,16 +131,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -417,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -435,175 +535,260 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.63</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.740097</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.70422799999999997</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.68475200000000003</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.75736599999999998</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.71135000000000004</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.72983100000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.72089599999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.70961600000000002</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.68886000000000003</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.67760200000000004</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.72021800000000002</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.69323999999999997</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.70418999999999998</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.69881400000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.74299800000000005</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.68089599999999995</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.63914199999999999</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.77693000000000001</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.687168</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.72575000000000001</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.70772699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.75772309807966198</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.71512100048725002</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.68739975049010804</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.78119316921712101</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.72085036794766899</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.74669832319335205</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.73440174264820202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.75725528775208995</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.71414088162537004</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.68592942434503601</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.78110445775116399</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.71982980315144696</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.74612320989746606</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.73362377470048201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>0.61</v>
-      </c>
-      <c r="D3">
-        <v>0.62</v>
-      </c>
-      <c r="E3">
-        <v>0.63</v>
-      </c>
-      <c r="F3">
-        <v>0.6</v>
-      </c>
-      <c r="G3">
-        <v>0.62</v>
-      </c>
-      <c r="H3">
-        <v>0.61</v>
-      </c>
-      <c r="I3">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0.74</v>
-      </c>
-      <c r="D5">
-        <v>0.7</v>
-      </c>
-      <c r="E5">
-        <v>0.69</v>
-      </c>
-      <c r="F5">
-        <v>0.75</v>
-      </c>
-      <c r="G5">
-        <v>0.71</v>
-      </c>
-      <c r="H5">
-        <v>0.73</v>
-      </c>
-      <c r="I5">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>0.71</v>
-      </c>
-      <c r="D6">
-        <v>0.69</v>
-      </c>
-      <c r="E6">
-        <v>0.67</v>
-      </c>
-      <c r="F6">
-        <v>0.73</v>
-      </c>
-      <c r="G6">
-        <v>0.69</v>
-      </c>
-      <c r="H6">
-        <v>0.71</v>
-      </c>
-      <c r="I6">
-        <v>0.69869999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>0.69</v>
-      </c>
-      <c r="D7">
-        <v>0.63</v>
-      </c>
-      <c r="E7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F7">
-        <v>0.75</v>
-      </c>
-      <c r="G7">
-        <v>0.62</v>
-      </c>
-      <c r="H7">
-        <v>0.68</v>
-      </c>
-      <c r="I7">
-        <v>0.65171999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update result table, remake plots
</commit_message>
<xml_diff>
--- a/Jerry/statistic.xlsx
+++ b/Jerry/statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\repo\MAST30034FinalProject\Jerry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E9BCD6-AFD0-4A5A-9108-3C5119A93C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E45A8F0-33F2-41BC-AB38-F3B03EA3DFE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9650" yWindow="3550" windowWidth="16820" windowHeight="10790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,12 +218,6 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -237,6 +231,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -520,7 +520,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -534,261 +534,261 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>0.61</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>0.62</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>0.63</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>0.6</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>0.62</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>0.61</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>0.61</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>0.740097</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>0.70422799999999997</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.68475200000000003</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>0.75736599999999998</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>0.71135000000000004</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>0.72983100000000001</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>0.72089599999999998</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.70961600000000002</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>0.68886000000000003</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.67760200000000004</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>0.72021800000000002</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>0.69323999999999997</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>0.70418999999999998</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>0.69881400000000005</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
-        <v>0.74299800000000005</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.68089599999999995</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.63914199999999999</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.77693000000000001</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.687168</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0.72575000000000001</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0.70772699999999999</v>
+      <c r="C6" s="4">
+        <v>0.74775100000000005</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.67009200000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.61404899999999996</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.79098800000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.67433699999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.72553800000000002</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.70212200000000002</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>0.75772309807966198</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>0.71512100048725002</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>0.68739975049010804</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>0.78119316921712101</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>0.72085036794766899</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>0.74669832319335205</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>0.73440174264820202</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>0.75725528775208995</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>0.71414088162537004</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>0.68592942434503601</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>0.78110445775116399</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>0.71982980315144696</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <v>0.74612320989746606</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>0.73362377470048201</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>